<commit_message>
Updated 12MW hub height (132->136). Updated OSW cost xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/examples/H2_Analysis/OSW_H2_sites_turbines_and_costs.xlsx
+++ b/examples/H2_Analysis/OSW_H2_sites_turbines_and_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriccobo\Documents\GitProjects\HOPP\examples\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52379F9F-172C-4CCB-958C-5C59EF4F7A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BA412F-19A2-422A-B7B3-CE071AE9219A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0BE0E57E-7BF2-4188-95EF-49DFC633BEBE}"/>
   </bookViews>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB30163-94D1-4EC7-AC79-39520D1CD789}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1438,13 +1438,13 @@
         <v>72</v>
       </c>
       <c r="B25" s="11">
-        <v>568</v>
+        <v>577</v>
       </c>
       <c r="C25" s="11">
         <v>1051</v>
       </c>
       <c r="D25" s="11">
-        <v>548</v>
+        <v>558</v>
       </c>
       <c r="E25" s="11">
         <v>1051</v>
@@ -1588,7 +1588,7 @@
         <v>77</v>
       </c>
       <c r="B33" s="11">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C33" s="11">
         <v>76</v>
@@ -1606,7 +1606,7 @@
         <v>78</v>
       </c>
       <c r="B34" s="11">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" s="8">
         <v>0</v>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B36" s="24">
         <f>SUM(B23:B35)</f>
-        <v>1376.5</v>
+        <v>1387.5</v>
       </c>
       <c r="C36" s="24">
         <f t="shared" ref="C36:E36" si="0">SUM(C23:C35)</f>
@@ -1655,7 +1655,7 @@
       </c>
       <c r="D36" s="24">
         <f t="shared" si="0"/>
-        <v>1362.7807884945144</v>
+        <v>1372.7807884945144</v>
       </c>
       <c r="E36" s="24">
         <f t="shared" si="0"/>
@@ -1695,7 +1695,7 @@
         <v>71</v>
       </c>
       <c r="E38" s="11">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F38" s="17"/>
     </row>
@@ -1704,7 +1704,7 @@
         <v>81</v>
       </c>
       <c r="B39" s="11">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C39" s="11">
         <v>220</v>
@@ -1740,7 +1740,7 @@
         <v>83</v>
       </c>
       <c r="B41" s="11">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C41" s="11">
         <v>153</v>
@@ -1776,11 +1776,11 @@
         <v>100</v>
       </c>
       <c r="B43" s="25">
-        <f>SUM(B37:B42)</f>
-        <v>532</v>
+        <f t="shared" ref="B43:E43" si="1">SUM(B37:B42)</f>
+        <v>534</v>
       </c>
       <c r="C43" s="25">
-        <f t="shared" ref="C43:E43" si="1">SUM(C37:C42)</f>
+        <f t="shared" si="1"/>
         <v>788</v>
       </c>
       <c r="D43" s="25">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="E43" s="25">
         <f t="shared" si="1"/>
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F43" s="31"/>
     </row>
@@ -1818,16 +1818,16 @@
         <v>85</v>
       </c>
       <c r="B45" s="28">
-        <v>3210</v>
+        <v>3221</v>
       </c>
       <c r="C45" s="28">
         <v>5332</v>
       </c>
       <c r="D45" s="28">
-        <v>3199</v>
+        <v>3209</v>
       </c>
       <c r="E45" s="28">
-        <v>4246</v>
+        <v>4244</v>
       </c>
       <c r="F45" s="33"/>
     </row>
@@ -1836,7 +1836,7 @@
         <v>67</v>
       </c>
       <c r="B46" s="30">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="30">
         <v>116</v>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="B48" s="2">
         <f>SUM(B36,B43,B44)</f>
-        <v>3208.5</v>
+        <v>3221.5</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" ref="C48:E48" si="2">SUM(C36,C43,C44)</f>
@@ -1873,11 +1873,11 @@
       </c>
       <c r="D48" s="2">
         <f t="shared" si="2"/>
-        <v>3199.7807884945141</v>
+        <v>3209.7807884945141</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" si="2"/>
-        <v>4247.0315080136716</v>
+        <v>4246.0315080136716</v>
       </c>
       <c r="F48" s="6"/>
     </row>
@@ -3717,12 +3717,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1b167cac-9da6-43f0-b7e7-4775de4a2f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9073c3f8-2855-48ea-b895-d99d76b52c59" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3903,20 +3905,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1b167cac-9da6-43f0-b7e7-4775de4a2f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9073c3f8-2855-48ea-b895-d99d76b52c59" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC3BB5E4-732B-4F6D-BBD7-58B22D237A2C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E5B756-34F6-4DD2-912D-8BE97B958C34}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="9073c3f8-2855-48ea-b895-d99d76b52c59"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1b167cac-9da6-43f0-b7e7-4775de4a2f66"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3941,18 +3950,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E5B756-34F6-4DD2-912D-8BE97B958C34}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC3BB5E4-732B-4F6D-BBD7-58B22D237A2C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9073c3f8-2855-48ea-b895-d99d76b52c59"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1b167cac-9da6-43f0-b7e7-4775de4a2f66"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated ORBIT spreadsheet with updated turbine component values from Shields et. al
</commit_message>
<xml_diff>
--- a/examples/H2_Analysis/OSW_H2_sites_turbines_and_costs.xlsx
+++ b/examples/H2_Analysis/OSW_H2_sites_turbines_and_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriccobo\Documents\GitProjects\HOPP\examples\H2_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BA412F-19A2-422A-B7B3-CE071AE9219A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282A34F7-D1CB-4C91-9819-CFDC860F844B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0BE0E57E-7BF2-4188-95EF-49DFC633BEBE}"/>
   </bookViews>
@@ -592,7 +592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -601,16 +601,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -649,13 +644,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -977,7 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB30163-94D1-4EC7-AC79-39520D1CD789}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
@@ -1007,7 +1002,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1015,37 +1010,37 @@
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1053,19 +1048,19 @@
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1073,19 +1068,19 @@
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1093,37 +1088,37 @@
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1131,125 +1126,125 @@
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="17"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="17"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="17"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1257,39 +1252,39 @@
       <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>0.55600000000000005</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>0.55400000000000005</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>0.53100000000000003</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="35">
         <v>0.44500000000000001</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="35">
         <v>0.49</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="35">
         <v>0.44500000000000001</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="35">
         <v>0.49</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="38" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1297,37 +1292,37 @@
       <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1335,29 +1330,25 @@
       <c r="A19" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="17"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
@@ -1375,99 +1366,99 @@
       <c r="E21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="37">
         <v>115</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="37">
         <v>92</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="37">
         <v>115</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="37">
         <v>92</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="38" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="12">
         <v>67</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="12">
         <v>169</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>66</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="12">
         <v>108</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="2">
         <v>90</v>
       </c>
-      <c r="C24" s="11">
-        <v>58</v>
-      </c>
-      <c r="D24" s="11">
+      <c r="C24" s="2">
+        <v>59</v>
+      </c>
+      <c r="D24" s="2">
         <v>85</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="2">
         <v>25</v>
       </c>
-      <c r="F24" s="17"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="2">
         <v>577</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="2">
         <v>1051</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="2">
         <v>558</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="2">
         <v>1051</v>
       </c>
-      <c r="F25" s="17"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="9">
         <v>0</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="2">
         <v>1288</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="9">
         <v>0</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="2">
         <v>523.03150801367201</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="14" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1475,37 +1466,37 @@
       <c r="A27" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="2">
         <v>233</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="2">
         <v>234</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="2">
         <v>234</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="2">
         <v>234</v>
       </c>
-      <c r="F27" s="17"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="2">
         <v>17.5</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="6">
         <v>0</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="2">
         <v>17.739999999999998</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="6">
         <v>0</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1513,73 +1504,73 @@
       <c r="A29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="2">
         <v>32</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="2">
         <v>42</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="2">
         <v>32.040788494514402</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="2">
         <v>36</v>
       </c>
-      <c r="F29" s="17"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="2">
         <v>178</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="2">
         <v>175</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="2">
         <v>178</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="2">
         <v>175</v>
       </c>
-      <c r="F30" s="17"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="2">
         <v>4</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="2">
         <v>5</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="2">
         <v>4</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="2">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="11">
+      <c r="B32" s="2">
         <v>38</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="6">
         <v>0</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="2">
         <v>44</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="6">
         <v>0</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1587,277 +1578,272 @@
       <c r="A33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="2">
         <v>55</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="2">
         <v>76</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="2">
         <v>56</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="2">
         <v>62</v>
       </c>
-      <c r="F33" s="17"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="2">
         <v>96</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="6">
         <v>0</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="2">
         <v>98</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="9">
         <v>0</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="17">
         <v>0</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="18">
         <v>145</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="17">
         <v>0</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="18">
         <v>93</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="19" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="24">
+      <c r="B36" s="21">
         <f>SUM(B23:B35)</f>
         <v>1387.5</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="21">
         <f t="shared" ref="C36:E36" si="0">SUM(C23:C35)</f>
-        <v>3243</v>
-      </c>
-      <c r="D36" s="24">
+        <v>3244</v>
+      </c>
+      <c r="D36" s="21">
         <f t="shared" si="0"/>
         <v>1372.7807884945144</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="21">
         <f t="shared" si="0"/>
         <v>2311.031508013672</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="28"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="12">
         <v>31</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="12">
         <v>52</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="12">
         <v>31</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="12">
         <v>42</v>
       </c>
-      <c r="F37" s="18"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="2">
         <v>69</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="2">
         <v>76</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="2">
         <v>71</v>
       </c>
-      <c r="E38" s="11">
-        <v>63</v>
-      </c>
-      <c r="F38" s="17"/>
+      <c r="E38" s="2">
+        <v>64</v>
+      </c>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="2">
         <v>133</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="2">
         <v>220</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="2">
         <v>132</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E39" s="2">
         <v>175</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="2">
         <v>131</v>
       </c>
-      <c r="C40" s="11">
-        <v>235</v>
-      </c>
-      <c r="D40" s="11">
+      <c r="C40" s="2">
+        <v>236</v>
+      </c>
+      <c r="D40" s="2">
         <v>130</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E40" s="2">
         <v>186</v>
       </c>
-      <c r="F40" s="17"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="2">
         <v>139</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="2">
         <v>153</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="2">
         <v>142</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E41" s="2">
         <v>127</v>
       </c>
-      <c r="F41" s="17"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="21">
+      <c r="B42" s="18">
         <v>31</v>
       </c>
-      <c r="C42" s="21">
+      <c r="C42" s="18">
         <v>52</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="18">
         <v>31</v>
       </c>
-      <c r="E42" s="21">
+      <c r="E42" s="18">
         <v>42</v>
       </c>
-      <c r="F42" s="22"/>
+      <c r="F42" s="19"/>
     </row>
     <row r="43" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="22">
         <f t="shared" ref="B43:E43" si="1">SUM(B37:B42)</f>
         <v>534</v>
       </c>
-      <c r="C43" s="25">
+      <c r="C43" s="22">
         <f t="shared" si="1"/>
-        <v>788</v>
-      </c>
-      <c r="D43" s="25">
+        <v>789</v>
+      </c>
+      <c r="D43" s="22">
         <f t="shared" si="1"/>
         <v>537</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="22">
         <f t="shared" si="1"/>
-        <v>635</v>
-      </c>
-      <c r="F43" s="31"/>
+        <v>636</v>
+      </c>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="42">
+      <c r="B44" s="39">
         <v>1300</v>
       </c>
-      <c r="C44" s="42">
+      <c r="C44" s="39">
         <v>1300</v>
       </c>
-      <c r="D44" s="42">
+      <c r="D44" s="39">
         <v>1300</v>
       </c>
-      <c r="E44" s="42">
+      <c r="E44" s="39">
         <v>1300</v>
       </c>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="29" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="28">
+      <c r="B45" s="25">
         <v>3221</v>
       </c>
-      <c r="C45" s="28">
+      <c r="C45" s="25">
         <v>5332</v>
       </c>
-      <c r="D45" s="28">
-        <v>3209</v>
-      </c>
-      <c r="E45" s="28">
-        <v>4244</v>
-      </c>
-      <c r="F45" s="33"/>
+      <c r="D45" s="25">
+        <v>3210</v>
+      </c>
+      <c r="E45" s="25">
+        <v>4246</v>
+      </c>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="27">
         <v>93</v>
       </c>
-      <c r="C46" s="30">
+      <c r="C46" s="27">
         <v>116</v>
       </c>
-      <c r="D46" s="30">
+      <c r="D46" s="27">
         <v>92</v>
       </c>
-      <c r="E46" s="30">
+      <c r="E46" s="27">
         <v>97</v>
       </c>
-      <c r="F46" s="34" t="s">
+      <c r="F46" s="31" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
@@ -1869,7 +1855,7 @@
       </c>
       <c r="C48" s="2">
         <f t="shared" ref="C48:E48" si="2">SUM(C36,C43,C44)</f>
-        <v>5331</v>
+        <v>5333</v>
       </c>
       <c r="D48" s="2">
         <f t="shared" si="2"/>
@@ -1877,9 +1863,8 @@
       </c>
       <c r="E48" s="2">
         <f t="shared" si="2"/>
-        <v>4246.0315080136716</v>
-      </c>
-      <c r="F48" s="6"/>
+        <v>4247.0315080136716</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1893,7 +1878,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1922,7 +1907,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1930,37 +1915,37 @@
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1968,19 +1953,19 @@
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1988,19 +1973,19 @@
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2008,37 +1993,37 @@
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2046,125 +2031,125 @@
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="17"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="17"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="17"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2172,39 +2157,39 @@
       <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>0.55600000000000005</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>0.55400000000000005</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>0.53100000000000003</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="35">
         <v>0.46100000000000002</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="35">
         <v>0.5</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="35">
         <v>0.46100000000000002</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="35">
         <v>0.5</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="38" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2212,37 +2197,37 @@
       <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2250,29 +2235,25 @@
       <c r="A19" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="17"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
@@ -2290,99 +2271,99 @@
       <c r="E21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="37">
         <v>103</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="37">
         <v>83</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="37">
         <v>103</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="37">
         <v>83</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="38" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="12">
         <v>62</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="12">
         <v>144</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>62</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="12">
         <v>95.6</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="2">
         <v>91</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="2">
         <v>59</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="2">
         <v>86</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="2">
         <v>26</v>
       </c>
-      <c r="F24" s="17"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="2">
         <v>561</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="2">
         <v>980</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="2">
         <v>543</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="2">
         <v>980</v>
       </c>
-      <c r="F25" s="17"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="9">
         <v>0</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="2">
         <v>1030</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="9">
         <v>0</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="2">
         <v>418</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="14" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2390,37 +2371,37 @@
       <c r="A27" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="2">
         <v>235</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="2">
         <v>235</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="2">
         <v>235</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="2">
         <v>235</v>
       </c>
-      <c r="F27" s="17"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="2">
         <v>17</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="6">
         <v>0</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="2">
         <v>17</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="6">
         <v>0</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2428,73 +2409,73 @@
       <c r="A29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="2">
         <v>26</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="2">
         <v>35</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="2">
         <v>26</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="2">
         <v>30</v>
       </c>
-      <c r="F29" s="17"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="2">
         <v>178</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="2">
         <v>175</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="2">
         <v>178</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="2">
         <v>175</v>
       </c>
-      <c r="F30" s="17"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="2">
         <v>4</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="2">
         <v>5</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="2">
         <v>4</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="2">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="11">
+      <c r="B32" s="2">
         <v>30</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="6">
         <v>0</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="2">
         <v>35</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="6">
         <v>0</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2502,277 +2483,272 @@
       <c r="A33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="2">
         <v>47</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="2">
         <v>61</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="2">
         <v>48</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="2">
         <v>50</v>
       </c>
-      <c r="F33" s="17"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="11">
-        <v>85</v>
-      </c>
-      <c r="C34" s="8">
+      <c r="B34" s="2">
+        <v>77</v>
+      </c>
+      <c r="C34" s="6">
         <v>0</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="2">
+        <v>79</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="12">
+      <c r="B35" s="17">
         <v>0</v>
       </c>
-      <c r="F34" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B35" s="20">
+      <c r="C35" s="18">
+        <v>116</v>
+      </c>
+      <c r="D35" s="17">
         <v>0</v>
       </c>
-      <c r="C35" s="21">
-        <v>116</v>
-      </c>
-      <c r="D35" s="20">
-        <v>0</v>
-      </c>
-      <c r="E35" s="21">
-        <v>73</v>
-      </c>
-      <c r="F35" s="22" t="s">
+      <c r="E35" s="18">
+        <v>75</v>
+      </c>
+      <c r="F35" s="19" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="24">
+      <c r="B36" s="21">
         <f>SUM(B23:B35)</f>
-        <v>1336</v>
-      </c>
-      <c r="C36" s="24">
+        <v>1328</v>
+      </c>
+      <c r="C36" s="21">
         <f t="shared" ref="C36:E36" si="0">SUM(C23:C35)</f>
         <v>2840</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="21">
         <f t="shared" si="0"/>
-        <v>1323</v>
-      </c>
-      <c r="E36" s="24">
+        <v>1313</v>
+      </c>
+      <c r="E36" s="21">
         <f t="shared" si="0"/>
-        <v>2086.6</v>
-      </c>
-      <c r="F36" s="31"/>
+        <v>2088.6</v>
+      </c>
+      <c r="F36" s="28"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="12">
         <v>30</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="12">
         <v>47</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="12">
         <v>30</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="12">
         <v>39</v>
       </c>
-      <c r="F37" s="18"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="2">
+        <v>62</v>
+      </c>
+      <c r="C38" s="2">
+        <v>67</v>
+      </c>
+      <c r="D38" s="2">
         <v>64</v>
       </c>
-      <c r="C38" s="11">
-        <v>67</v>
-      </c>
-      <c r="D38" s="11">
-        <v>65</v>
-      </c>
-      <c r="E38" s="11">
+      <c r="E38" s="2">
         <v>57</v>
       </c>
-      <c r="F38" s="17"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="2">
         <v>129</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="2">
         <v>199</v>
       </c>
-      <c r="D39" s="11">
-        <v>129</v>
-      </c>
-      <c r="E39" s="11">
+      <c r="D39" s="2">
+        <v>128</v>
+      </c>
+      <c r="E39" s="2">
         <v>163</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="2">
         <v>130</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="2">
         <v>214</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="2">
         <v>128</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E40" s="2">
         <v>175</v>
       </c>
-      <c r="F40" s="17"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="2">
+        <v>124</v>
+      </c>
+      <c r="C41" s="2">
+        <v>134</v>
+      </c>
+      <c r="D41" s="2">
         <v>127</v>
       </c>
-      <c r="C41" s="11">
-        <v>134</v>
-      </c>
-      <c r="D41" s="11">
-        <v>131</v>
-      </c>
-      <c r="E41" s="11">
+      <c r="E41" s="2">
         <v>114</v>
       </c>
-      <c r="F41" s="17"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="21">
+      <c r="B42" s="18">
         <v>30</v>
       </c>
-      <c r="C42" s="21">
+      <c r="C42" s="18">
         <v>47</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="18">
         <v>30</v>
       </c>
-      <c r="E42" s="21">
+      <c r="E42" s="18">
         <v>39</v>
       </c>
-      <c r="F42" s="22"/>
+      <c r="F42" s="19"/>
     </row>
     <row r="43" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="22">
         <f t="shared" ref="B43:E43" si="1">SUM(B37:B42)</f>
-        <v>510</v>
-      </c>
-      <c r="C43" s="25">
+        <v>505</v>
+      </c>
+      <c r="C43" s="22">
         <f t="shared" si="1"/>
         <v>708</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="22">
         <f t="shared" si="1"/>
-        <v>513</v>
-      </c>
-      <c r="E43" s="25">
+        <v>507</v>
+      </c>
+      <c r="E43" s="22">
         <f t="shared" si="1"/>
         <v>587</v>
       </c>
-      <c r="F43" s="31"/>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="42">
+      <c r="B44" s="39">
         <v>1300</v>
       </c>
-      <c r="C44" s="42">
+      <c r="C44" s="39">
         <v>1300</v>
       </c>
-      <c r="D44" s="42">
+      <c r="D44" s="39">
         <v>1300</v>
       </c>
-      <c r="E44" s="42">
+      <c r="E44" s="39">
         <v>1300</v>
       </c>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="29" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="28">
-        <v>3146</v>
-      </c>
-      <c r="C45" s="28">
+      <c r="B45" s="25">
+        <v>3134</v>
+      </c>
+      <c r="C45" s="25">
         <v>4848</v>
       </c>
-      <c r="D45" s="28">
-        <v>3137</v>
-      </c>
-      <c r="E45" s="28">
-        <v>3971</v>
-      </c>
-      <c r="F45" s="33"/>
+      <c r="D45" s="25">
+        <v>3121</v>
+      </c>
+      <c r="E45" s="25">
+        <v>3973</v>
+      </c>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="27">
         <v>85</v>
       </c>
-      <c r="C46" s="30">
-        <v>103</v>
-      </c>
-      <c r="D46" s="30">
+      <c r="C46" s="27">
+        <v>104</v>
+      </c>
+      <c r="D46" s="27">
         <v>85</v>
       </c>
-      <c r="E46" s="30">
+      <c r="E46" s="27">
         <v>88</v>
       </c>
-      <c r="F46" s="34" t="s">
+      <c r="F46" s="31" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
@@ -2780,7 +2756,7 @@
       </c>
       <c r="B48" s="2">
         <f>SUM(B36,B43,B44)</f>
-        <v>3146</v>
+        <v>3133</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" ref="C48:E48" si="2">SUM(C36,C43,C44)</f>
@@ -2788,13 +2764,12 @@
       </c>
       <c r="D48" s="2">
         <f t="shared" si="2"/>
-        <v>3136</v>
+        <v>3120</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" si="2"/>
-        <v>3973.6</v>
-      </c>
-      <c r="F48" s="6"/>
+        <v>3975.6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2806,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9538386-45E8-4ECC-B6E1-C95D6C0E1F2E}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2836,7 +2811,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2844,37 +2819,37 @@
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2882,19 +2857,19 @@
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2902,19 +2877,19 @@
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2922,37 +2897,37 @@
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2960,125 +2935,125 @@
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="17"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="17"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="17"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3086,39 +3061,39 @@
       <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>0.55600000000000005</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>0.55400000000000005</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>0.53100000000000003</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="35">
         <v>0.46800000000000003</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="35">
         <v>0.51</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="35">
         <v>0.46800000000000003</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="35">
         <v>0.51</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="38" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3126,37 +3101,37 @@
       <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="33">
         <v>7.6399999999999996E-2</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3164,29 +3139,25 @@
       <c r="A19" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="17"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
@@ -3204,99 +3175,99 @@
       <c r="E21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="37">
         <v>97</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="37">
         <v>78</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="37">
         <v>97</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="37">
         <v>78</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="38" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="12">
         <v>59</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="12">
         <v>128</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>59</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="12">
         <v>87</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="2">
         <v>91</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="2">
         <v>59</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="2">
         <v>86</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="2">
         <v>26</v>
       </c>
-      <c r="F24" s="17"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="2">
         <v>548</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="2">
         <v>942</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="2">
         <v>531</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="2">
         <v>942</v>
       </c>
-      <c r="F25" s="17"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="9">
         <v>0</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="2">
         <v>859</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="9">
         <v>0</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="2">
         <v>349</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="14" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3304,37 +3275,37 @@
       <c r="A27" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="2">
         <v>235</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="2">
         <v>235</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="2">
         <v>235</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="2">
         <v>235</v>
       </c>
-      <c r="F27" s="17"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="2">
         <v>16</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="6">
         <v>0</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="2">
         <v>16</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="6">
         <v>0</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3342,73 +3313,73 @@
       <c r="A29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="2">
         <v>23</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="2">
         <v>30</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="2">
         <v>23</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="2">
         <v>25</v>
       </c>
-      <c r="F29" s="17"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="2">
         <v>178</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="2">
         <v>175</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="2">
         <v>178</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="2">
         <v>175</v>
       </c>
-      <c r="F30" s="17"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="2">
         <v>4</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="2">
         <v>5</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="2">
         <v>4</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="2">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="11">
+      <c r="B32" s="2">
         <v>25</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="6">
         <v>0</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="2">
         <v>29</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="6">
         <v>0</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3416,277 +3387,272 @@
       <c r="A33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="2">
         <v>39</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="2">
         <v>51</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="2">
         <v>41</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="2">
         <v>42</v>
       </c>
-      <c r="F33" s="17"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="2">
         <v>72</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="6">
         <v>0</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="2">
         <v>75</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="9">
         <v>0</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="17">
         <v>0</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="18">
         <v>97</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="17">
         <v>0</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="18">
         <v>62</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="19" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="24">
+      <c r="B36" s="21">
         <f>SUM(B23:B35)</f>
         <v>1290</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="21">
         <f t="shared" ref="C36:E36" si="0">SUM(C23:C35)</f>
         <v>2581</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="21">
         <f t="shared" si="0"/>
         <v>1277</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="21">
         <f t="shared" si="0"/>
         <v>1947</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="28"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="12">
         <v>30</v>
       </c>
-      <c r="C37" s="15">
+      <c r="C37" s="12">
         <v>44</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="12">
         <v>30</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="12">
         <v>37</v>
       </c>
-      <c r="F37" s="18"/>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="11">
-        <v>59</v>
-      </c>
-      <c r="C38" s="11">
+      <c r="B38" s="2">
+        <v>58</v>
+      </c>
+      <c r="C38" s="2">
         <v>61</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="2">
         <v>60</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E38" s="2">
         <v>53</v>
       </c>
-      <c r="F38" s="17"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="2">
         <v>126</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="2">
         <v>186</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="2">
         <v>126</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E39" s="2">
         <v>156</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="2">
         <v>129</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="2">
         <v>201</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="2">
         <v>127</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E40" s="2">
         <v>168</v>
       </c>
-      <c r="F40" s="17"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="2">
         <v>117</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="2">
         <v>123</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="2">
         <v>120</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E41" s="2">
         <v>105</v>
       </c>
-      <c r="F41" s="17"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="21">
+      <c r="B42" s="18">
         <v>30</v>
       </c>
-      <c r="C42" s="21">
+      <c r="C42" s="18">
         <v>44</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="18">
         <v>30</v>
       </c>
-      <c r="E42" s="21">
+      <c r="E42" s="18">
         <v>37</v>
       </c>
-      <c r="F42" s="22"/>
+      <c r="F42" s="19"/>
     </row>
     <row r="43" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="22">
         <f>SUM(B37:B42)</f>
-        <v>491</v>
-      </c>
-      <c r="C43" s="25">
+        <v>490</v>
+      </c>
+      <c r="C43" s="22">
         <f t="shared" ref="C43:E43" si="1">SUM(C37:C42)</f>
         <v>659</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="22">
         <f t="shared" si="1"/>
         <v>493</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="22">
         <f t="shared" si="1"/>
         <v>556</v>
       </c>
-      <c r="F43" s="31"/>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="42">
+      <c r="B44" s="39">
         <v>1300</v>
       </c>
-      <c r="C44" s="42">
+      <c r="C44" s="39">
         <v>1300</v>
       </c>
-      <c r="D44" s="42">
+      <c r="D44" s="39">
         <v>1300</v>
       </c>
-      <c r="E44" s="42">
+      <c r="E44" s="39">
         <v>1300</v>
       </c>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="29" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="28">
-        <v>3079</v>
-      </c>
-      <c r="C45" s="28">
+      <c r="B45" s="25">
+        <v>3080</v>
+      </c>
+      <c r="C45" s="25">
         <v>4540</v>
       </c>
-      <c r="D45" s="28">
+      <c r="D45" s="25">
         <v>3069</v>
       </c>
-      <c r="E45" s="28">
-        <v>3802</v>
-      </c>
-      <c r="F45" s="33"/>
+      <c r="E45" s="25">
+        <v>3803</v>
+      </c>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="27">
         <v>81</v>
       </c>
-      <c r="C46" s="30">
+      <c r="C46" s="27">
         <v>95</v>
       </c>
-      <c r="D46" s="30">
+      <c r="D46" s="27">
         <v>81</v>
       </c>
-      <c r="E46" s="30">
+      <c r="E46" s="27">
         <v>83</v>
       </c>
-      <c r="F46" s="34" t="s">
+      <c r="F46" s="31" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
@@ -3694,7 +3660,7 @@
       </c>
       <c r="B48" s="2">
         <f>SUM(B36,B43,B44)</f>
-        <v>3081</v>
+        <v>3080</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" ref="C48:E48" si="2">SUM(C36,C43,C44)</f>
@@ -3708,7 +3674,6 @@
         <f t="shared" si="2"/>
         <v>3803</v>
       </c>
-      <c r="F48" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3717,14 +3682,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1b167cac-9da6-43f0-b7e7-4775de4a2f66">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9073c3f8-2855-48ea-b895-d99d76b52c59" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3905,27 +3868,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1b167cac-9da6-43f0-b7e7-4775de4a2f66">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9073c3f8-2855-48ea-b895-d99d76b52c59" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E5B756-34F6-4DD2-912D-8BE97B958C34}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC3BB5E4-732B-4F6D-BBD7-58B22D237A2C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9073c3f8-2855-48ea-b895-d99d76b52c59"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1b167cac-9da6-43f0-b7e7-4775de4a2f66"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3950,9 +3906,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC3BB5E4-732B-4F6D-BBD7-58B22D237A2C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9E5B756-34F6-4DD2-912D-8BE97B958C34}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="9073c3f8-2855-48ea-b895-d99d76b52c59"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1b167cac-9da6-43f0-b7e7-4775de4a2f66"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>